<commit_message>
update calendar sheet update
</commit_message>
<xml_diff>
--- a/public/sample-calendar.xlsx
+++ b/public/sample-calendar.xlsx
@@ -7,11 +7,16 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="x0Np/5Zr3DbXsnQIBcE5M0coQKljdItF8BpHOHkgHfI="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>reason</t>
   </si>
@@ -25,25 +30,16 @@
     <t>type</t>
   </si>
   <si>
-    <t>International Mother Language Day</t>
+    <t>New Year Holiday</t>
   </si>
   <si>
     <t>holiday</t>
   </si>
   <si>
-    <t>Shab-e-Barat</t>
-  </si>
-  <si>
-    <t>Durga Puja</t>
+    <t>Team Meating</t>
   </si>
   <si>
     <t>event</t>
-  </si>
-  <si>
-    <t>Victory Day (Bangladesh)</t>
-  </si>
-  <si>
-    <t>Christmas Day</t>
   </si>
 </sst>
 </file>
@@ -81,10 +77,10 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="14" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -324,82 +320,43 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
-        <v>46071.0</v>
+      <c r="B2" s="3">
+        <v>45658.0</v>
       </c>
-      <c r="C2" s="2">
-        <v>46088.0</v>
+      <c r="C2" s="3">
+        <v>45658.0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
-        <v>46071.0</v>
+      <c r="B3" s="3">
+        <v>45689.0</v>
       </c>
-      <c r="C3" s="2">
-        <v>46090.0</v>
+      <c r="C3" s="3">
+        <v>45689.0</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2">
-        <v>46071.0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>46081.0</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C4" s="4"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2">
-        <v>46071.0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>46071.0</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
+    <row r="5" ht="15.75" customHeight="1"/>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="C6" s="4"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2">
-        <v>46071.0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>46142.0</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="C7" s="4"/>
-    </row>
+    <row r="7" ht="15.75" customHeight="1"/>
     <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="C9" s="4"/>
-    </row>
+    <row r="9" ht="15.75" customHeight="1"/>
     <row r="10" ht="15.75" customHeight="1"/>
     <row r="11" ht="15.75" customHeight="1"/>
     <row r="12" ht="15.75" customHeight="1"/>
@@ -1388,9 +1345,6 @@
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>